<commit_message>
replace example.org with nzlum.landcareresearch.co.nz namespace
</commit_message>
<xml_diff>
--- a/classification-systems/nzlum/build/management_practices.xlsx
+++ b/classification-systems/nzlum/build/management_practices.xlsx
@@ -484,14 +484,10 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>barn laid</t>
-        </is>
-      </c>
-      <c r="C2" s="2" t="inlineStr">
-        <is>
-          <t>https://example.org/landuse/management_practice/barn_laid</t>
-        </is>
-      </c>
+          <t xml:space="preserve">milking walk through </t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="inlineStr"/>
       <c r="D2" s="2" t="inlineStr"/>
       <c r="E2" s="2" t="inlineStr"/>
       <c r="F2" s="2" t="inlineStr"/>
@@ -500,14 +496,10 @@
       <c r="A3" s="2" t="n"/>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>caged</t>
-        </is>
-      </c>
-      <c r="C3" s="2" t="inlineStr">
-        <is>
-          <t>https://example.org/landuse/management_practice/caged</t>
-        </is>
-      </c>
+          <t>milking rotary</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="inlineStr"/>
       <c r="D3" s="2" t="inlineStr"/>
       <c r="E3" s="2" t="inlineStr"/>
       <c r="F3" s="2" t="inlineStr"/>
@@ -516,14 +508,10 @@
       <c r="A4" s="2" t="n"/>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>free range</t>
-        </is>
-      </c>
-      <c r="C4" s="2" t="inlineStr">
-        <is>
-          <t>https://example.org/landuse/management_practice/free_range</t>
-        </is>
-      </c>
+          <t>milking hand</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="inlineStr"/>
       <c r="D4" s="2" t="inlineStr"/>
       <c r="E4" s="2" t="inlineStr"/>
       <c r="F4" s="2" t="inlineStr"/>
@@ -532,14 +520,10 @@
       <c r="A5" s="2" t="n"/>
       <c r="B5" s="2" t="inlineStr">
         <is>
-          <t>milking hand</t>
-        </is>
-      </c>
-      <c r="C5" s="2" t="inlineStr">
-        <is>
-          <t>https://example.org/landuse/management_practice/milking_hand</t>
-        </is>
-      </c>
+          <t>caged</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr"/>
       <c r="D5" s="2" t="inlineStr"/>
       <c r="E5" s="2" t="inlineStr"/>
       <c r="F5" s="2" t="inlineStr"/>
@@ -548,14 +532,10 @@
       <c r="A6" s="2" t="n"/>
       <c r="B6" s="2" t="inlineStr">
         <is>
-          <t>milking herringbone</t>
-        </is>
-      </c>
-      <c r="C6" s="2" t="inlineStr">
-        <is>
-          <t>https://example.org/landuse/management_practice/milking_herringbone</t>
-        </is>
-      </c>
+          <t>free range</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="inlineStr"/>
       <c r="D6" s="2" t="inlineStr"/>
       <c r="E6" s="2" t="inlineStr"/>
       <c r="F6" s="2" t="inlineStr"/>
@@ -564,14 +544,10 @@
       <c r="A7" s="2" t="n"/>
       <c r="B7" s="2" t="inlineStr">
         <is>
-          <t>milking rotary</t>
-        </is>
-      </c>
-      <c r="C7" s="2" t="inlineStr">
-        <is>
-          <t>https://example.org/landuse/management_practice/milking_rotary</t>
-        </is>
-      </c>
+          <t>barn laid</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="inlineStr"/>
       <c r="D7" s="2" t="inlineStr"/>
       <c r="E7" s="2" t="inlineStr"/>
       <c r="F7" s="2" t="inlineStr"/>
@@ -580,14 +556,10 @@
       <c r="A8" s="2" t="n"/>
       <c r="B8" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">milking walk through </t>
-        </is>
-      </c>
-      <c r="C8" s="2" t="inlineStr">
-        <is>
-          <t>https://example.org/landuse/management_practice/milking_walk_through</t>
-        </is>
-      </c>
+          <t>milking herringbone</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="inlineStr"/>
       <c r="D8" s="2" t="inlineStr"/>
       <c r="E8" s="2" t="inlineStr"/>
       <c r="F8" s="2" t="inlineStr"/>
@@ -600,14 +572,10 @@
       </c>
       <c r="B9" s="2" t="inlineStr">
         <is>
-          <t>biodynamic</t>
-        </is>
-      </c>
-      <c r="C9" s="2" t="inlineStr">
-        <is>
-          <t>https://example.org/landuse/management_practice/biodynamic</t>
-        </is>
-      </c>
+          <t>tillage conservation</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="inlineStr"/>
       <c r="D9" s="2" t="inlineStr"/>
       <c r="E9" s="2" t="inlineStr"/>
       <c r="F9" s="2" t="inlineStr"/>
@@ -616,14 +584,10 @@
       <c r="A10" s="2" t="n"/>
       <c r="B10" s="2" t="inlineStr">
         <is>
-          <t>contour banks</t>
-        </is>
-      </c>
-      <c r="C10" s="2" t="inlineStr">
-        <is>
-          <t>https://example.org/landuse/management_practice/contour_banks</t>
-        </is>
-      </c>
+          <t>cropping rotational</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="inlineStr"/>
       <c r="D10" s="2" t="inlineStr"/>
       <c r="E10" s="2" t="inlineStr"/>
       <c r="F10" s="2" t="inlineStr"/>
@@ -632,14 +596,10 @@
       <c r="A11" s="2" t="n"/>
       <c r="B11" s="2" t="inlineStr">
         <is>
-          <t>controlled traffic farming</t>
-        </is>
-      </c>
-      <c r="C11" s="2" t="inlineStr">
-        <is>
-          <t>https://example.org/landuse/management_practice/controlled_traffic_farming</t>
-        </is>
-      </c>
+          <t>residues mulched</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="inlineStr"/>
       <c r="D11" s="2" t="inlineStr"/>
       <c r="E11" s="2" t="inlineStr"/>
       <c r="F11" s="2" t="inlineStr"/>
@@ -648,14 +608,10 @@
       <c r="A12" s="2" t="n"/>
       <c r="B12" s="2" t="inlineStr">
         <is>
-          <t>crop pasture rotation</t>
-        </is>
-      </c>
-      <c r="C12" s="2" t="inlineStr">
-        <is>
-          <t>https://example.org/landuse/management_practice/crop_pasture_rotation</t>
-        </is>
-      </c>
+          <t>organic</t>
+        </is>
+      </c>
+      <c r="C12" s="2" t="inlineStr"/>
       <c r="D12" s="2" t="inlineStr"/>
       <c r="E12" s="2" t="inlineStr"/>
       <c r="F12" s="2" t="inlineStr"/>
@@ -664,14 +620,10 @@
       <c r="A13" s="2" t="n"/>
       <c r="B13" s="2" t="inlineStr">
         <is>
-          <t>cropping continuous</t>
-        </is>
-      </c>
-      <c r="C13" s="2" t="inlineStr">
-        <is>
-          <t>https://example.org/landuse/management_practice/cropping_continuous</t>
-        </is>
-      </c>
+          <t>residues heavily grazed</t>
+        </is>
+      </c>
+      <c r="C13" s="2" t="inlineStr"/>
       <c r="D13" s="2" t="inlineStr"/>
       <c r="E13" s="2" t="inlineStr"/>
       <c r="F13" s="2" t="inlineStr"/>
@@ -680,14 +632,10 @@
       <c r="A14" s="2" t="n"/>
       <c r="B14" s="2" t="inlineStr">
         <is>
-          <t>cropping cover</t>
-        </is>
-      </c>
-      <c r="C14" s="2" t="inlineStr">
-        <is>
-          <t>https://example.org/landuse/management_practice/cropping_cover</t>
-        </is>
-      </c>
+          <t>cropping multiple</t>
+        </is>
+      </c>
+      <c r="C14" s="2" t="inlineStr"/>
       <c r="D14" s="2" t="inlineStr"/>
       <c r="E14" s="2" t="inlineStr"/>
       <c r="F14" s="2" t="inlineStr"/>
@@ -696,14 +644,10 @@
       <c r="A15" s="2" t="n"/>
       <c r="B15" s="2" t="inlineStr">
         <is>
-          <t>cropping multiple</t>
-        </is>
-      </c>
-      <c r="C15" s="2" t="inlineStr">
-        <is>
-          <t>https://example.org/landuse/management_practice/cropping_multiple</t>
-        </is>
-      </c>
+          <t>biodynamic</t>
+        </is>
+      </c>
+      <c r="C15" s="2" t="inlineStr"/>
       <c r="D15" s="2" t="inlineStr"/>
       <c r="E15" s="2" t="inlineStr"/>
       <c r="F15" s="2" t="inlineStr"/>
@@ -712,14 +656,10 @@
       <c r="A16" s="2" t="n"/>
       <c r="B16" s="2" t="inlineStr">
         <is>
-          <t>cropping opportunistic</t>
-        </is>
-      </c>
-      <c r="C16" s="2" t="inlineStr">
-        <is>
-          <t>https://example.org/landuse/management_practice/cropping_opportunistic</t>
-        </is>
-      </c>
+          <t>cropping cover</t>
+        </is>
+      </c>
+      <c r="C16" s="2" t="inlineStr"/>
       <c r="D16" s="2" t="inlineStr"/>
       <c r="E16" s="2" t="inlineStr"/>
       <c r="F16" s="2" t="inlineStr"/>
@@ -728,14 +668,10 @@
       <c r="A17" s="2" t="n"/>
       <c r="B17" s="2" t="inlineStr">
         <is>
-          <t>cropping rotational</t>
-        </is>
-      </c>
-      <c r="C17" s="2" t="inlineStr">
-        <is>
-          <t>https://example.org/landuse/management_practice/cropping_rotational</t>
-        </is>
-      </c>
+          <t>crop pasture rotation</t>
+        </is>
+      </c>
+      <c r="C17" s="2" t="inlineStr"/>
       <c r="D17" s="2" t="inlineStr"/>
       <c r="E17" s="2" t="inlineStr"/>
       <c r="F17" s="2" t="inlineStr"/>
@@ -744,14 +680,10 @@
       <c r="A18" s="2" t="n"/>
       <c r="B18" s="2" t="inlineStr">
         <is>
-          <t>cropping row alley</t>
-        </is>
-      </c>
-      <c r="C18" s="2" t="inlineStr">
-        <is>
-          <t>https://example.org/landuse/management_practice/cropping_row_alley</t>
-        </is>
-      </c>
+          <t>fallow chemical</t>
+        </is>
+      </c>
+      <c r="C18" s="2" t="inlineStr"/>
       <c r="D18" s="2" t="inlineStr"/>
       <c r="E18" s="2" t="inlineStr"/>
       <c r="F18" s="2" t="inlineStr"/>
@@ -760,14 +692,10 @@
       <c r="A19" s="2" t="n"/>
       <c r="B19" s="2" t="inlineStr">
         <is>
-          <t>cropping strip</t>
-        </is>
-      </c>
-      <c r="C19" s="2" t="inlineStr">
-        <is>
-          <t>https://example.org/landuse/management_practice/cropping_strip</t>
-        </is>
-      </c>
+          <t>tillage conventional</t>
+        </is>
+      </c>
+      <c r="C19" s="2" t="inlineStr"/>
       <c r="D19" s="2" t="inlineStr"/>
       <c r="E19" s="2" t="inlineStr"/>
       <c r="F19" s="2" t="inlineStr"/>
@@ -776,14 +704,10 @@
       <c r="A20" s="2" t="n"/>
       <c r="B20" s="2" t="inlineStr">
         <is>
-          <t>fallow chemical</t>
-        </is>
-      </c>
-      <c r="C20" s="2" t="inlineStr">
-        <is>
-          <t>https://example.org/landuse/management_practice/fallow_chemical</t>
-        </is>
-      </c>
+          <t>precision agriculture</t>
+        </is>
+      </c>
+      <c r="C20" s="2" t="inlineStr"/>
       <c r="D20" s="2" t="inlineStr"/>
       <c r="E20" s="2" t="inlineStr"/>
       <c r="F20" s="2" t="inlineStr"/>
@@ -792,14 +716,10 @@
       <c r="A21" s="2" t="n"/>
       <c r="B21" s="2" t="inlineStr">
         <is>
-          <t>fallow mechanical</t>
-        </is>
-      </c>
-      <c r="C21" s="2" t="inlineStr">
-        <is>
-          <t>https://example.org/landuse/management_practice/fallow_mechanical</t>
-        </is>
-      </c>
+          <t>residues intact</t>
+        </is>
+      </c>
+      <c r="C21" s="2" t="inlineStr"/>
       <c r="D21" s="2" t="inlineStr"/>
       <c r="E21" s="2" t="inlineStr"/>
       <c r="F21" s="2" t="inlineStr"/>
@@ -808,14 +728,10 @@
       <c r="A22" s="2" t="n"/>
       <c r="B22" s="2" t="inlineStr">
         <is>
-          <t>organic</t>
-        </is>
-      </c>
-      <c r="C22" s="2" t="inlineStr">
-        <is>
-          <t>https://example.org/landuse/management_practice/organic</t>
-        </is>
-      </c>
+          <t>controlled traffic farming</t>
+        </is>
+      </c>
+      <c r="C22" s="2" t="inlineStr"/>
       <c r="D22" s="2" t="inlineStr"/>
       <c r="E22" s="2" t="inlineStr"/>
       <c r="F22" s="2" t="inlineStr"/>
@@ -824,14 +740,10 @@
       <c r="A23" s="2" t="n"/>
       <c r="B23" s="2" t="inlineStr">
         <is>
-          <t>pasture cropping</t>
-        </is>
-      </c>
-      <c r="C23" s="2" t="inlineStr">
-        <is>
-          <t>https://example.org/landuse/management_practice/pasture_cropping</t>
-        </is>
-      </c>
+          <t>residues burnt</t>
+        </is>
+      </c>
+      <c r="C23" s="2" t="inlineStr"/>
       <c r="D23" s="2" t="inlineStr"/>
       <c r="E23" s="2" t="inlineStr"/>
       <c r="F23" s="2" t="inlineStr"/>
@@ -840,14 +752,10 @@
       <c r="A24" s="2" t="n"/>
       <c r="B24" s="2" t="inlineStr">
         <is>
-          <t>precision agriculture</t>
-        </is>
-      </c>
-      <c r="C24" s="2" t="inlineStr">
-        <is>
-          <t>https://example.org/landuse/management_practice/precision_agriculture</t>
-        </is>
-      </c>
+          <t>cropping opportunistic</t>
+        </is>
+      </c>
+      <c r="C24" s="2" t="inlineStr"/>
       <c r="D24" s="2" t="inlineStr"/>
       <c r="E24" s="2" t="inlineStr"/>
       <c r="F24" s="2" t="inlineStr"/>
@@ -856,14 +764,10 @@
       <c r="A25" s="2" t="n"/>
       <c r="B25" s="2" t="inlineStr">
         <is>
-          <t>residues baled</t>
-        </is>
-      </c>
-      <c r="C25" s="2" t="inlineStr">
-        <is>
-          <t>https://example.org/landuse/management_practice/residues_baled</t>
-        </is>
-      </c>
+          <t>contour banks</t>
+        </is>
+      </c>
+      <c r="C25" s="2" t="inlineStr"/>
       <c r="D25" s="2" t="inlineStr"/>
       <c r="E25" s="2" t="inlineStr"/>
       <c r="F25" s="2" t="inlineStr"/>
@@ -872,14 +776,10 @@
       <c r="A26" s="2" t="n"/>
       <c r="B26" s="2" t="inlineStr">
         <is>
-          <t>residues burnt</t>
-        </is>
-      </c>
-      <c r="C26" s="2" t="inlineStr">
-        <is>
-          <t>https://example.org/landuse/management_practice/residues_burnt</t>
-        </is>
-      </c>
+          <t>fallow mechanical</t>
+        </is>
+      </c>
+      <c r="C26" s="2" t="inlineStr"/>
       <c r="D26" s="2" t="inlineStr"/>
       <c r="E26" s="2" t="inlineStr"/>
       <c r="F26" s="2" t="inlineStr"/>
@@ -888,14 +788,10 @@
       <c r="A27" s="2" t="n"/>
       <c r="B27" s="2" t="inlineStr">
         <is>
-          <t>residues heavily grazed</t>
-        </is>
-      </c>
-      <c r="C27" s="2" t="inlineStr">
-        <is>
-          <t>https://example.org/landuse/management_practice/residues_heavily_grazed</t>
-        </is>
-      </c>
+          <t>cropping continuous</t>
+        </is>
+      </c>
+      <c r="C27" s="2" t="inlineStr"/>
       <c r="D27" s="2" t="inlineStr"/>
       <c r="E27" s="2" t="inlineStr"/>
       <c r="F27" s="2" t="inlineStr"/>
@@ -904,14 +800,10 @@
       <c r="A28" s="2" t="n"/>
       <c r="B28" s="2" t="inlineStr">
         <is>
-          <t>residues incorporated</t>
-        </is>
-      </c>
-      <c r="C28" s="2" t="inlineStr">
-        <is>
-          <t>https://example.org/landuse/management_practice/residues_incorporated</t>
-        </is>
-      </c>
+          <t>pasture cropping</t>
+        </is>
+      </c>
+      <c r="C28" s="2" t="inlineStr"/>
       <c r="D28" s="2" t="inlineStr"/>
       <c r="E28" s="2" t="inlineStr"/>
       <c r="F28" s="2" t="inlineStr"/>
@@ -920,14 +812,10 @@
       <c r="A29" s="2" t="n"/>
       <c r="B29" s="2" t="inlineStr">
         <is>
-          <t>residues intact</t>
-        </is>
-      </c>
-      <c r="C29" s="2" t="inlineStr">
-        <is>
-          <t>https://example.org/landuse/management_practice/residues_intact</t>
-        </is>
-      </c>
+          <t>cropping strip</t>
+        </is>
+      </c>
+      <c r="C29" s="2" t="inlineStr"/>
       <c r="D29" s="2" t="inlineStr"/>
       <c r="E29" s="2" t="inlineStr"/>
       <c r="F29" s="2" t="inlineStr"/>
@@ -936,14 +824,10 @@
       <c r="A30" s="2" t="n"/>
       <c r="B30" s="2" t="inlineStr">
         <is>
-          <t>residues mulched</t>
-        </is>
-      </c>
-      <c r="C30" s="2" t="inlineStr">
-        <is>
-          <t>https://example.org/landuse/management_practice/residues_mulched</t>
-        </is>
-      </c>
+          <t>residues incorporated</t>
+        </is>
+      </c>
+      <c r="C30" s="2" t="inlineStr"/>
       <c r="D30" s="2" t="inlineStr"/>
       <c r="E30" s="2" t="inlineStr"/>
       <c r="F30" s="2" t="inlineStr"/>
@@ -952,14 +836,10 @@
       <c r="A31" s="2" t="n"/>
       <c r="B31" s="2" t="inlineStr">
         <is>
-          <t>tillage conservation</t>
-        </is>
-      </c>
-      <c r="C31" s="2" t="inlineStr">
-        <is>
-          <t>https://example.org/landuse/management_practice/tillage_conservation</t>
-        </is>
-      </c>
+          <t>cropping row alley</t>
+        </is>
+      </c>
+      <c r="C31" s="2" t="inlineStr"/>
       <c r="D31" s="2" t="inlineStr"/>
       <c r="E31" s="2" t="inlineStr"/>
       <c r="F31" s="2" t="inlineStr"/>
@@ -968,14 +848,10 @@
       <c r="A32" s="2" t="n"/>
       <c r="B32" s="2" t="inlineStr">
         <is>
-          <t>tillage conventional</t>
-        </is>
-      </c>
-      <c r="C32" s="2" t="inlineStr">
-        <is>
-          <t>https://example.org/landuse/management_practice/tillage_conventional</t>
-        </is>
-      </c>
+          <t>residues baled</t>
+        </is>
+      </c>
+      <c r="C32" s="2" t="inlineStr"/>
       <c r="D32" s="2" t="inlineStr"/>
       <c r="E32" s="2" t="inlineStr"/>
       <c r="F32" s="2" t="inlineStr"/>
@@ -988,29 +864,13 @@
       </c>
       <c r="B33" s="2" t="inlineStr">
         <is>
-          <t>grazing rotational</t>
-        </is>
-      </c>
-      <c r="C33" s="2" t="inlineStr">
-        <is>
-          <t>https://example.org/landuse/management_practice/grazing_rotational</t>
-        </is>
-      </c>
-      <c r="D33" s="2" t="inlineStr">
-        <is>
-          <t>Moving livestock between paddocks in regular sequence to permit the recovery and growth of the pasture plants after grazing.</t>
-        </is>
-      </c>
-      <c r="E33" s="2" t="inlineStr">
-        <is>
-          <t>Stocking rates per paddock are higher than under set stocking.</t>
-        </is>
-      </c>
-      <c r="F33" s="2" t="inlineStr">
-        <is>
-          <t>Also cell grazing.</t>
-        </is>
-      </c>
+          <t>grazing tactical</t>
+        </is>
+      </c>
+      <c r="C33" s="2" t="inlineStr"/>
+      <c r="D33" s="2" t="inlineStr"/>
+      <c r="E33" s="2" t="inlineStr"/>
+      <c r="F33" s="2" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" s="2" t="n"/>
@@ -1019,11 +879,7 @@
           <t>grazing set stocking</t>
         </is>
       </c>
-      <c r="C34" s="2" t="inlineStr">
-        <is>
-          <t>https://example.org/landuse/management_practice/grazing_set_stocking</t>
-        </is>
-      </c>
+      <c r="C34" s="2" t="inlineStr"/>
       <c r="D34" s="2" t="inlineStr"/>
       <c r="E34" s="2" t="inlineStr"/>
       <c r="F34" s="2" t="inlineStr"/>
@@ -1032,17 +888,25 @@
       <c r="A35" s="2" t="n"/>
       <c r="B35" s="2" t="inlineStr">
         <is>
-          <t>grazing tactical</t>
-        </is>
-      </c>
-      <c r="C35" s="2" t="inlineStr">
-        <is>
-          <t>https://example.org/landuse/management_practice/grazing_tactical</t>
-        </is>
-      </c>
-      <c r="D35" s="2" t="inlineStr"/>
-      <c r="E35" s="2" t="inlineStr"/>
-      <c r="F35" s="2" t="inlineStr"/>
+          <t>grazing rotational</t>
+        </is>
+      </c>
+      <c r="C35" s="2" t="inlineStr"/>
+      <c r="D35" s="2" t="inlineStr">
+        <is>
+          <t>Moving livestock between paddocks in regular sequence to permit the recovery and growth of the pasture plants after grazing.</t>
+        </is>
+      </c>
+      <c r="E35" s="2" t="inlineStr">
+        <is>
+          <t>Stocking rates per paddock are higher than under set stocking.</t>
+        </is>
+      </c>
+      <c r="F35" s="2" t="inlineStr">
+        <is>
+          <t>Also cell grazing.</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="inlineStr">
@@ -1052,14 +916,10 @@
       </c>
       <c r="B36" s="2" t="inlineStr">
         <is>
-          <t>free standing</t>
-        </is>
-      </c>
-      <c r="C36" s="2" t="inlineStr">
-        <is>
-          <t>https://example.org/landuse/management_practice/free_standing</t>
-        </is>
-      </c>
+          <t>mulching/matting</t>
+        </is>
+      </c>
+      <c r="C36" s="2" t="inlineStr"/>
       <c r="D36" s="2" t="inlineStr"/>
       <c r="E36" s="2" t="inlineStr"/>
       <c r="F36" s="2" t="inlineStr"/>
@@ -1068,14 +928,10 @@
       <c r="A37" s="2" t="n"/>
       <c r="B37" s="2" t="inlineStr">
         <is>
-          <t>fully protected</t>
-        </is>
-      </c>
-      <c r="C37" s="2" t="inlineStr">
-        <is>
-          <t>https://example.org/landuse/management_practice/fully_protected</t>
-        </is>
-      </c>
+          <t>open growing</t>
+        </is>
+      </c>
+      <c r="C37" s="2" t="inlineStr"/>
       <c r="D37" s="2" t="inlineStr"/>
       <c r="E37" s="2" t="inlineStr"/>
       <c r="F37" s="2" t="inlineStr"/>
@@ -1087,11 +943,7 @@
           <t>hedgerow</t>
         </is>
       </c>
-      <c r="C38" s="2" t="inlineStr">
-        <is>
-          <t>https://example.org/landuse/management_practice/hedgerow</t>
-        </is>
-      </c>
+      <c r="C38" s="2" t="inlineStr"/>
       <c r="D38" s="2" t="inlineStr"/>
       <c r="E38" s="2" t="inlineStr"/>
       <c r="F38" s="2" t="inlineStr"/>
@@ -1100,14 +952,10 @@
       <c r="A39" s="2" t="n"/>
       <c r="B39" s="2" t="inlineStr">
         <is>
-          <t>mulching/matting</t>
-        </is>
-      </c>
-      <c r="C39" s="2" t="inlineStr">
-        <is>
-          <t>https://example.org/landuse/management_practice/mulching_matting</t>
-        </is>
-      </c>
+          <t>free standing</t>
+        </is>
+      </c>
+      <c r="C39" s="2" t="inlineStr"/>
       <c r="D39" s="2" t="inlineStr"/>
       <c r="E39" s="2" t="inlineStr"/>
       <c r="F39" s="2" t="inlineStr"/>
@@ -1116,14 +964,10 @@
       <c r="A40" s="2" t="n"/>
       <c r="B40" s="2" t="inlineStr">
         <is>
-          <t>open growing</t>
-        </is>
-      </c>
-      <c r="C40" s="2" t="inlineStr">
-        <is>
-          <t>https://example.org/landuse/management_practice/open_growing</t>
-        </is>
-      </c>
+          <t>fully protected</t>
+        </is>
+      </c>
+      <c r="C40" s="2" t="inlineStr"/>
       <c r="D40" s="2" t="inlineStr"/>
       <c r="E40" s="2" t="inlineStr"/>
       <c r="F40" s="2" t="inlineStr"/>
@@ -1132,14 +976,10 @@
       <c r="A41" s="2" t="n"/>
       <c r="B41" s="2" t="inlineStr">
         <is>
-          <t>semi-protected</t>
-        </is>
-      </c>
-      <c r="C41" s="2" t="inlineStr">
-        <is>
-          <t>https://example.org/landuse/management_practice/semi_protected</t>
-        </is>
-      </c>
+          <t>trellis/espalier</t>
+        </is>
+      </c>
+      <c r="C41" s="2" t="inlineStr"/>
       <c r="D41" s="2" t="inlineStr"/>
       <c r="E41" s="2" t="inlineStr"/>
       <c r="F41" s="2" t="inlineStr"/>
@@ -1148,14 +988,10 @@
       <c r="A42" s="2" t="n"/>
       <c r="B42" s="2" t="inlineStr">
         <is>
-          <t>trellis/espalier</t>
-        </is>
-      </c>
-      <c r="C42" s="2" t="inlineStr">
-        <is>
-          <t>https://example.org/landuse/management_practice/trellis_espalier</t>
-        </is>
-      </c>
+          <t>semi-protected</t>
+        </is>
+      </c>
+      <c r="C42" s="2" t="inlineStr"/>
       <c r="D42" s="2" t="inlineStr"/>
       <c r="E42" s="2" t="inlineStr"/>
       <c r="F42" s="2" t="inlineStr"/>
@@ -1168,23 +1004,19 @@
       </c>
       <c r="B43" s="2" t="inlineStr">
         <is>
-          <t>irrigation drip</t>
-        </is>
-      </c>
-      <c r="C43" s="2" t="inlineStr">
-        <is>
-          <t>https://example.org/landuse/management_practice/irrigation_drip</t>
-        </is>
-      </c>
+          <t>irrigation surface</t>
+        </is>
+      </c>
+      <c r="C43" s="2" t="inlineStr"/>
       <c r="D43" s="2" t="inlineStr">
         <is>
-          <t>Irrigation system that applies water to the soil very slowly through tubes/tapes either above or below the soil surface.</t>
+          <t>Water is applied to the land by allowing it to flow by simple gravity before infiltrating. Under furrow irrigation, small parallel channels carry water to irrigate the crop with the crop usually grown on the ridges between the furrows.</t>
         </is>
       </c>
       <c r="E43" s="2" t="inlineStr"/>
       <c r="F43" s="2" t="inlineStr">
         <is>
-          <t>Also trickle irrigation.</t>
+          <t>Also flood/furrow irrigation.</t>
         </is>
       </c>
     </row>
@@ -1195,11 +1027,7 @@
           <t>irrigation spray</t>
         </is>
       </c>
-      <c r="C44" s="2" t="inlineStr">
-        <is>
-          <t>https://example.org/landuse/management_practice/irrigation_spray</t>
-        </is>
-      </c>
+      <c r="C44" s="2" t="inlineStr"/>
       <c r="D44" s="2" t="inlineStr">
         <is>
           <t>Irrigation system that sprays water into the air allowing it to fall on the plants and soil much like natural rainfall.</t>
@@ -1216,23 +1044,19 @@
       <c r="A45" s="2" t="n"/>
       <c r="B45" s="2" t="inlineStr">
         <is>
-          <t>irrigation surface</t>
-        </is>
-      </c>
-      <c r="C45" s="2" t="inlineStr">
-        <is>
-          <t>https://example.org/landuse/management_practice/irrigation_surface</t>
-        </is>
-      </c>
+          <t>irrigation drip</t>
+        </is>
+      </c>
+      <c r="C45" s="2" t="inlineStr"/>
       <c r="D45" s="2" t="inlineStr">
         <is>
-          <t>Water is applied to the land by allowing it to flow by simple gravity before infiltrating. Under furrow irrigation, small parallel channels carry water to irrigate the crop with the crop usually grown on the ridges between the furrows.</t>
+          <t>Irrigation system that applies water to the soil very slowly through tubes/tapes either above or below the soil surface.</t>
         </is>
       </c>
       <c r="E45" s="2" t="inlineStr"/>
       <c r="F45" s="2" t="inlineStr">
         <is>
-          <t>Also flood/furrow irrigation.</t>
+          <t>Also trickle irrigation.</t>
         </is>
       </c>
     </row>
@@ -1244,14 +1068,10 @@
       </c>
       <c r="B46" s="2" t="inlineStr">
         <is>
-          <t>biodynamic</t>
-        </is>
-      </c>
-      <c r="C46" s="2" t="inlineStr">
-        <is>
-          <t>https://example.org/landuse/management_practice/biodynamic</t>
-        </is>
-      </c>
+          <t>crop pasture rotation</t>
+        </is>
+      </c>
+      <c r="C46" s="2" t="inlineStr"/>
       <c r="D46" s="2" t="inlineStr"/>
       <c r="E46" s="2" t="inlineStr"/>
       <c r="F46" s="2" t="inlineStr"/>
@@ -1260,14 +1080,10 @@
       <c r="A47" s="2" t="n"/>
       <c r="B47" s="2" t="inlineStr">
         <is>
-          <t>crop pasture rotation</t>
-        </is>
-      </c>
-      <c r="C47" s="2" t="inlineStr">
-        <is>
-          <t>https://example.org/landuse/management_practice/crop_pasture_rotation</t>
-        </is>
-      </c>
+          <t>precision agriculture</t>
+        </is>
+      </c>
+      <c r="C47" s="2" t="inlineStr"/>
       <c r="D47" s="2" t="inlineStr"/>
       <c r="E47" s="2" t="inlineStr"/>
       <c r="F47" s="2" t="inlineStr"/>
@@ -1279,11 +1095,7 @@
           <t>organic</t>
         </is>
       </c>
-      <c r="C48" s="2" t="inlineStr">
-        <is>
-          <t>https://example.org/landuse/management_practice/organic</t>
-        </is>
-      </c>
+      <c r="C48" s="2" t="inlineStr"/>
       <c r="D48" s="2" t="inlineStr"/>
       <c r="E48" s="2" t="inlineStr"/>
       <c r="F48" s="2" t="inlineStr"/>
@@ -1292,14 +1104,10 @@
       <c r="A49" s="2" t="n"/>
       <c r="B49" s="2" t="inlineStr">
         <is>
-          <t>pasture cropping</t>
-        </is>
-      </c>
-      <c r="C49" s="2" t="inlineStr">
-        <is>
-          <t>https://example.org/landuse/management_practice/pasture_cropping</t>
-        </is>
-      </c>
+          <t>biodynamic</t>
+        </is>
+      </c>
+      <c r="C49" s="2" t="inlineStr"/>
       <c r="D49" s="2" t="inlineStr"/>
       <c r="E49" s="2" t="inlineStr"/>
       <c r="F49" s="2" t="inlineStr"/>
@@ -1308,14 +1116,10 @@
       <c r="A50" s="2" t="n"/>
       <c r="B50" s="2" t="inlineStr">
         <is>
-          <t>precision agriculture</t>
-        </is>
-      </c>
-      <c r="C50" s="2" t="inlineStr">
-        <is>
-          <t>https://example.org/landuse/management_practice/precision_agriculture</t>
-        </is>
-      </c>
+          <t>pasture cropping</t>
+        </is>
+      </c>
+      <c r="C50" s="2" t="inlineStr"/>
       <c r="D50" s="2" t="inlineStr"/>
       <c r="E50" s="2" t="inlineStr"/>
       <c r="F50" s="2" t="inlineStr"/>

</xml_diff>